<commit_message>
changed example file, and added exercises
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -630,7 +630,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y504"/>
+  <dimension ref="A1:Y505"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B322" activePane="bottomRight" state="frozen"/>
@@ -23273,7 +23273,7 @@
         <v>4.0476838336840668</v>
       </c>
       <c r="Q345" s="6">
-        <v>2.380921703730186</v>
+        <v>2.3809217037301855</v>
       </c>
       <c r="R345" s="6">
         <v>49.294313471202614</v>
@@ -23301,51 +23301,111 @@
       </c>
     </row>
     <row r="346" spans="1:25" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A346" s="17"/>
-      <c r="B346" s="19"/>
-      <c r="C346" s="21"/>
-      <c r="D346" s="19"/>
-      <c r="E346" s="21"/>
-      <c r="F346" s="19"/>
-      <c r="G346" s="21"/>
-      <c r="H346" s="19"/>
-      <c r="I346" s="21"/>
-      <c r="J346" s="19"/>
-      <c r="K346" s="21"/>
-      <c r="L346" s="19"/>
-      <c r="M346" s="21"/>
-      <c r="N346" s="5"/>
-      <c r="O346" s="22"/>
-      <c r="P346" s="5"/>
-      <c r="Q346" s="22"/>
-      <c r="R346" s="22"/>
-      <c r="S346" s="22"/>
-      <c r="T346" s="22"/>
-      <c r="U346" s="22"/>
-      <c r="V346" s="22"/>
-      <c r="W346" s="22"/>
-      <c r="X346" s="22"/>
-      <c r="Y346" s="22"/>
+      <c r="A346" s="17">
+        <v>45383</v>
+      </c>
+      <c r="B346" s="19">
+        <v>5745.5309999999999</v>
+      </c>
+      <c r="C346" s="20">
+        <v>11093.629000000001</v>
+      </c>
+      <c r="D346" s="19">
+        <v>43097.915999999997</v>
+      </c>
+      <c r="E346" s="20">
+        <v>25658.307989636698</v>
+      </c>
+      <c r="F346" s="19">
+        <v>16312.409121699398</v>
+      </c>
+      <c r="G346" s="20">
+        <v>4685.95</v>
+      </c>
+      <c r="H346" s="19">
+        <v>11626.459121699398</v>
+      </c>
+      <c r="I346" s="20">
+        <v>9345.8988679372978</v>
+      </c>
+      <c r="J346" s="19">
+        <v>17439.60764550426</v>
+      </c>
+      <c r="K346" s="20">
+        <v>38411.965635140958</v>
+      </c>
+      <c r="L346" s="19">
+        <v>4138.8810000000003</v>
+      </c>
+      <c r="M346" s="20">
+        <v>1055.0586488699998</v>
+      </c>
+      <c r="N346" s="5">
+        <v>45.401497572802526</v>
+      </c>
+      <c r="O346" s="6">
+        <v>48.2540961495584</v>
+      </c>
+      <c r="P346" s="5">
+        <v>3.8849249420545786</v>
+      </c>
+      <c r="Q346" s="6">
+        <v>2.3128867920169944</v>
+      </c>
+      <c r="R346" s="6"/>
+      <c r="S346" s="6"/>
+      <c r="T346" s="11"/>
+      <c r="U346" s="11"/>
+      <c r="V346" s="11"/>
+      <c r="W346" s="6"/>
+      <c r="X346" s="6"/>
+      <c r="Y346" s="6"/>
     </row>
     <row r="347" spans="1:25" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A347" s="18"/>
+      <c r="A347" s="17"/>
+      <c r="B347" s="19"/>
+      <c r="C347" s="21"/>
+      <c r="D347" s="19"/>
+      <c r="E347" s="21"/>
+      <c r="F347" s="19"/>
+      <c r="G347" s="21"/>
+      <c r="H347" s="19"/>
+      <c r="I347" s="21"/>
+      <c r="J347" s="19"/>
+      <c r="K347" s="21"/>
+      <c r="L347" s="19"/>
+      <c r="M347" s="21"/>
+      <c r="N347" s="5"/>
+      <c r="O347" s="22"/>
+      <c r="P347" s="5"/>
+      <c r="Q347" s="22"/>
+      <c r="R347" s="22"/>
+      <c r="S347" s="22"/>
+      <c r="T347" s="22"/>
+      <c r="U347" s="22"/>
+      <c r="V347" s="22"/>
+      <c r="W347" s="22"/>
+      <c r="X347" s="22"/>
+      <c r="Y347" s="22"/>
     </row>
     <row r="348" spans="1:25" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A348" s="1"/>
-      <c r="B348" s="12" t="s">
+      <c r="A348" s="18"/>
+    </row>
+    <row r="349" spans="1:25" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A349" s="1"/>
+      <c r="B349" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="349" spans="1:25" ht="36.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A349" s="1"/>
-      <c r="B349" s="24" t="s">
+    <row r="350" spans="1:25" ht="36.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A350" s="1"/>
+      <c r="B350" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C349" s="24"/>
-      <c r="D349" s="24"/>
-      <c r="E349" s="24"/>
-    </row>
-    <row r="350" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C350" s="24"/>
+      <c r="D350" s="24"/>
+      <c r="E350" s="24"/>
+    </row>
     <row r="351" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="352" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -23500,10 +23560,11 @@
     <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:U1"/>
-    <mergeCell ref="B349:E349"/>
+    <mergeCell ref="B350:E350"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23531,7 +23592,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9455EDA8-AE8A-4212-B068-FCCA23F38CB4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3549689-4D04-4306-97D7-BA2D4D18266D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>